<commit_message>
implemented complete flow with two types of payment methods
</commit_message>
<xml_diff>
--- a/src/test/resources/testDataFile.xlsx
+++ b/src/test/resources/testDataFile.xlsx
@@ -4,7 +4,6 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="PURCHASEDRESS" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="PURCHASEDRESS2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -23,7 +22,7 @@
     <t>dress_name</t>
   </si>
   <si>
-    <t>TC01_CUSTOMER_PLACES_ORDER_FROM_SEARCH</t>
+    <t>TC01_CUSTOMER_PLACES_ORDER_BY_CHEQUE</t>
   </si>
   <si>
     <t>Y</t>
@@ -32,7 +31,7 @@
     <t>Printed Chiffon Dress</t>
   </si>
   <si>
-    <t>TC02_CUSTOMER_PLACES_ORDER_FROM_SEARCH</t>
+    <t>TC02_CUSTOMER_PLACES_ORDER_BY_BANK_WIRE</t>
   </si>
   <si>
     <t>Printed Summer Dress</t>
@@ -87,10 +86,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -298,7 +293,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="40.43"/>
+    <col customWidth="1" min="1" max="1" width="50.14"/>
     <col customWidth="1" min="3" max="3" width="19.14"/>
   </cols>
   <sheetData>
@@ -314,7 +309,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -331,49 +326,7 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="49.86"/>
-    <col customWidth="1" min="2" max="2" width="4.57"/>
-    <col customWidth="1" min="3" max="3" width="19.14"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>